<commit_message>
files added for AK Jain
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="61">
   <si>
     <t>Rank</t>
   </si>
@@ -824,25 +824,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>744</c:v>
+                  <c:v>898</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>166</c:v>
+                  <c:v>442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>43</c:v>
+                  <c:v>188</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5</c:v>
+                  <c:v>62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2</c:v>
+                  <c:v>7</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0</c:v>
@@ -851,7 +851,7 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1409,8 +1409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:AJ58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="H76" sqref="H76"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1564,70 +1564,90 @@
       <c r="G5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="I5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="J5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="K5" s="6"/>
+      <c r="K5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="L5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="M5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="N5" s="6"/>
+      <c r="N5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="O5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="P5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="Q5" s="6"/>
+      <c r="Q5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="R5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="S5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="T5" s="6"/>
+      <c r="T5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="U5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="V5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="W5" s="6"/>
+      <c r="W5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="X5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="Y5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="Z5" s="6"/>
+      <c r="Z5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="AA5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="AB5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AC5" s="6"/>
+      <c r="AC5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="AD5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="AE5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AF5" s="6"/>
+      <c r="AF5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="AG5" s="23" t="s">
         <v>59</v>
       </c>
       <c r="AH5" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="AI5" s="6"/>
+      <c r="AI5" s="6" t="s">
+        <v>60</v>
+      </c>
       <c r="AJ5" s="23" t="s">
         <v>59</v>
       </c>
@@ -1759,7 +1779,10 @@
         <f t="shared" ref="D7:D55" si="0">SUM(G7,J7,M7,P7,S7,V7,Y7,AB7,AE7,AH7)</f>
         <v>915</v>
       </c>
-      <c r="E7" s="34"/>
+      <c r="E7" s="34">
+        <f>H7+K7+N7+Q7+T7+W7+Z7+AC7+AF7+AI7</f>
+        <v>673</v>
+      </c>
       <c r="F7" s="17">
         <f t="shared" ref="F7:F55" si="1">SUM(I7,L7,O7,R7,U7,X7,AA7,AD7,AG7,AJ7)</f>
         <v>586</v>
@@ -1767,46 +1790,70 @@
       <c r="G7">
         <v>220</v>
       </c>
+      <c r="H7">
+        <v>154</v>
+      </c>
       <c r="I7" s="17">
         <v>153</v>
       </c>
       <c r="J7">
         <v>428</v>
       </c>
+      <c r="K7">
+        <v>276</v>
+      </c>
       <c r="L7" s="17">
         <v>231</v>
       </c>
       <c r="M7">
         <v>199</v>
       </c>
+      <c r="N7">
+        <v>145</v>
+      </c>
       <c r="O7" s="17">
         <v>146</v>
       </c>
       <c r="P7">
         <v>37</v>
       </c>
+      <c r="Q7">
+        <v>57</v>
+      </c>
       <c r="R7" s="17">
         <v>25</v>
       </c>
       <c r="S7">
         <v>24</v>
       </c>
+      <c r="T7">
+        <v>34</v>
+      </c>
       <c r="U7" s="17">
         <v>20</v>
       </c>
       <c r="V7">
         <v>5</v>
       </c>
+      <c r="W7">
+        <v>5</v>
+      </c>
       <c r="X7" s="17">
         <v>4</v>
       </c>
       <c r="Y7">
         <v>2</v>
       </c>
+      <c r="Z7">
+        <v>1</v>
+      </c>
       <c r="AA7" s="17">
         <v>0</v>
       </c>
       <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7">
         <v>0</v>
       </c>
       <c r="AD7" s="17">
@@ -1815,11 +1862,17 @@
       <c r="AE7">
         <v>0</v>
       </c>
+      <c r="AF7">
+        <v>0</v>
+      </c>
       <c r="AG7" s="17">
         <v>1</v>
       </c>
       <c r="AH7">
         <v>0</v>
+      </c>
+      <c r="AI7">
+        <v>1</v>
       </c>
       <c r="AJ7" s="17">
         <v>4</v>
@@ -1839,7 +1892,10 @@
         <f t="shared" si="0"/>
         <v>904</v>
       </c>
-      <c r="E8" s="34"/>
+      <c r="E8" s="34">
+        <f t="shared" ref="E8:E55" si="2">H8+K8+N8+Q8+T8+W8+Z8+AC8+AF8+AI8</f>
+        <v>0</v>
+      </c>
       <c r="F8" s="17">
         <f t="shared" si="1"/>
         <v>749</v>
@@ -1919,7 +1975,10 @@
         <f t="shared" si="0"/>
         <v>645</v>
       </c>
-      <c r="E9" s="34"/>
+      <c r="E9" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F9" s="17">
         <f t="shared" si="1"/>
         <v>605</v>
@@ -1999,7 +2058,10 @@
         <f t="shared" si="0"/>
         <v>474</v>
       </c>
-      <c r="E10" s="34"/>
+      <c r="E10" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F10" s="17">
         <f t="shared" si="1"/>
         <v>503</v>
@@ -2079,7 +2141,10 @@
         <f t="shared" si="0"/>
         <v>809</v>
       </c>
-      <c r="E11" s="34"/>
+      <c r="E11" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F11" s="17">
         <f t="shared" si="1"/>
         <v>714</v>
@@ -2159,7 +2224,10 @@
         <f t="shared" si="0"/>
         <v>719</v>
       </c>
-      <c r="E12" s="34"/>
+      <c r="E12" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F12" s="17">
         <f t="shared" si="1"/>
         <v>477</v>
@@ -2239,7 +2307,10 @@
         <f t="shared" si="0"/>
         <v>766</v>
       </c>
-      <c r="E13" s="34"/>
+      <c r="E13" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F13" s="17">
         <f t="shared" si="1"/>
         <v>751</v>
@@ -2319,7 +2390,10 @@
         <f t="shared" si="0"/>
         <v>522</v>
       </c>
-      <c r="E14" s="34"/>
+      <c r="E14" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F14" s="17">
         <f t="shared" si="1"/>
         <v>439</v>
@@ -2399,7 +2473,10 @@
         <f t="shared" si="0"/>
         <v>601</v>
       </c>
-      <c r="E15" s="34"/>
+      <c r="E15" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F15" s="17">
         <f t="shared" si="1"/>
         <v>499</v>
@@ -2479,7 +2556,10 @@
         <f t="shared" si="0"/>
         <v>959</v>
       </c>
-      <c r="E16" s="34"/>
+      <c r="E16" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F16" s="17">
         <f t="shared" si="1"/>
         <v>849</v>
@@ -2559,7 +2639,10 @@
         <f t="shared" si="0"/>
         <v>411</v>
       </c>
-      <c r="E17" s="34"/>
+      <c r="E17" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F17" s="17">
         <f t="shared" si="1"/>
         <v>495</v>
@@ -2639,7 +2722,10 @@
         <f t="shared" si="0"/>
         <v>505</v>
       </c>
-      <c r="E18" s="34"/>
+      <c r="E18" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F18" s="17">
         <f t="shared" si="1"/>
         <v>419</v>
@@ -2719,7 +2805,10 @@
         <f t="shared" si="0"/>
         <v>1154</v>
       </c>
-      <c r="E19" s="34"/>
+      <c r="E19" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F19" s="17">
         <f t="shared" si="1"/>
         <v>438</v>
@@ -2799,7 +2888,10 @@
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="E20" s="34"/>
+      <c r="E20" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F20" s="17">
         <f t="shared" si="1"/>
         <v>208</v>
@@ -2879,7 +2971,10 @@
         <f t="shared" si="0"/>
         <v>992</v>
       </c>
-      <c r="E21" s="34"/>
+      <c r="E21" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F21" s="17">
         <f t="shared" si="1"/>
         <v>932</v>
@@ -2959,7 +3054,10 @@
         <f t="shared" si="0"/>
         <v>1899</v>
       </c>
-      <c r="E22" s="34"/>
+      <c r="E22" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F22" s="17">
         <f t="shared" si="1"/>
         <v>975</v>
@@ -3039,7 +3137,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E23" s="34"/>
+      <c r="E23" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F23" s="17">
         <f t="shared" si="1"/>
         <v>473</v>
@@ -3109,7 +3210,10 @@
         <f t="shared" si="0"/>
         <v>506</v>
       </c>
-      <c r="E24" s="34"/>
+      <c r="E24" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F24" s="17">
         <f t="shared" si="1"/>
         <v>631</v>
@@ -3199,7 +3303,10 @@
         <f t="shared" si="0"/>
         <v>679</v>
       </c>
-      <c r="E25" s="34"/>
+      <c r="E25" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F25" s="17">
         <f t="shared" si="1"/>
         <v>508</v>
@@ -3289,7 +3396,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E26" s="34"/>
+      <c r="E26" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F26" s="17">
         <f t="shared" si="1"/>
         <v>614</v>
@@ -3359,7 +3469,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E27" s="34"/>
+      <c r="E27" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F27" s="17">
         <f t="shared" si="1"/>
         <v>533</v>
@@ -3429,7 +3542,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E28" s="34"/>
+      <c r="E28" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F28" s="17">
         <f t="shared" si="1"/>
         <v>790</v>
@@ -3499,7 +3615,10 @@
         <f t="shared" si="0"/>
         <v>446</v>
       </c>
-      <c r="E29" s="34"/>
+      <c r="E29" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F29" s="17">
         <f t="shared" si="1"/>
         <v>327</v>
@@ -3589,7 +3708,10 @@
         <f t="shared" si="0"/>
         <v>426</v>
       </c>
-      <c r="E30" s="34"/>
+      <c r="E30" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F30" s="17">
         <f t="shared" si="1"/>
         <v>448</v>
@@ -3679,7 +3801,10 @@
         <f t="shared" si="0"/>
         <v>797</v>
       </c>
-      <c r="E31" s="34"/>
+      <c r="E31" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F31" s="17">
         <f t="shared" si="1"/>
         <v>544</v>
@@ -3769,7 +3894,10 @@
         <f t="shared" si="0"/>
         <v>358</v>
       </c>
-      <c r="E32" s="34"/>
+      <c r="E32" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F32" s="17">
         <f t="shared" si="1"/>
         <v>270</v>
@@ -3859,7 +3987,10 @@
         <f t="shared" si="0"/>
         <v>515</v>
       </c>
-      <c r="E33" s="34"/>
+      <c r="E33" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F33" s="17">
         <f t="shared" si="1"/>
         <v>445</v>
@@ -3949,7 +4080,10 @@
         <f t="shared" si="0"/>
         <v>516</v>
       </c>
-      <c r="E34" s="34"/>
+      <c r="E34" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F34" s="17">
         <f t="shared" si="1"/>
         <v>740</v>
@@ -4039,7 +4173,10 @@
         <f t="shared" si="0"/>
         <v>1055</v>
       </c>
-      <c r="E35" s="34"/>
+      <c r="E35" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F35" s="17">
         <f t="shared" si="1"/>
         <v>997</v>
@@ -4129,7 +4266,10 @@
         <f t="shared" si="0"/>
         <v>563</v>
       </c>
-      <c r="E36" s="34"/>
+      <c r="E36" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F36" s="17">
         <f t="shared" si="1"/>
         <v>421</v>
@@ -4219,7 +4359,10 @@
         <f t="shared" si="0"/>
         <v>553</v>
       </c>
-      <c r="E37" s="34"/>
+      <c r="E37" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F37" s="17">
         <f t="shared" si="1"/>
         <v>397</v>
@@ -4309,7 +4452,10 @@
         <f t="shared" si="0"/>
         <v>599</v>
       </c>
-      <c r="E38" s="34"/>
+      <c r="E38" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F38" s="17">
         <f t="shared" si="1"/>
         <v>501</v>
@@ -4399,7 +4545,10 @@
         <f t="shared" si="0"/>
         <v>366</v>
       </c>
-      <c r="E39" s="34"/>
+      <c r="E39" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F39" s="17">
         <f t="shared" si="1"/>
         <v>314</v>
@@ -4489,7 +4638,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E40" s="34"/>
+      <c r="E40" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F40" s="17">
         <f t="shared" si="1"/>
         <v>630</v>
@@ -4559,7 +4711,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E41" s="34"/>
+      <c r="E41" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F41" s="17">
         <f t="shared" si="1"/>
         <v>618</v>
@@ -4629,7 +4784,10 @@
         <f t="shared" si="0"/>
         <v>3549</v>
       </c>
-      <c r="E42" s="34"/>
+      <c r="E42" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F42" s="17">
         <f t="shared" si="1"/>
         <v>671</v>
@@ -4719,7 +4877,10 @@
         <f t="shared" si="0"/>
         <v>613</v>
       </c>
-      <c r="E43" s="34"/>
+      <c r="E43" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F43" s="17">
         <f t="shared" si="1"/>
         <v>464</v>
@@ -4809,7 +4970,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E44" s="34"/>
+      <c r="E44" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F44" s="17">
         <f t="shared" si="1"/>
         <v>402</v>
@@ -4879,7 +5043,10 @@
         <f t="shared" si="0"/>
         <v>361</v>
       </c>
-      <c r="E45" s="34"/>
+      <c r="E45" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F45" s="17">
         <f t="shared" si="1"/>
         <v>402</v>
@@ -4969,7 +5136,10 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="E46" s="34"/>
+      <c r="E46" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F46" s="17">
         <f t="shared" si="1"/>
         <v>930</v>
@@ -5039,7 +5209,10 @@
         <f t="shared" si="0"/>
         <v>3195</v>
       </c>
-      <c r="E47" s="34"/>
+      <c r="E47" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F47" s="17">
         <f t="shared" si="1"/>
         <v>593</v>
@@ -5129,7 +5302,10 @@
         <f t="shared" si="0"/>
         <v>650</v>
       </c>
-      <c r="E48" s="34"/>
+      <c r="E48" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F48" s="17">
         <f t="shared" si="1"/>
         <v>480</v>
@@ -5219,7 +5395,10 @@
         <f t="shared" si="0"/>
         <v>899</v>
       </c>
-      <c r="E49" s="34"/>
+      <c r="E49" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F49" s="17">
         <f t="shared" si="1"/>
         <v>615</v>
@@ -5309,7 +5488,10 @@
         <f t="shared" si="0"/>
         <v>565</v>
       </c>
-      <c r="E50" s="34"/>
+      <c r="E50" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F50" s="17">
         <f t="shared" si="1"/>
         <v>551</v>
@@ -5399,7 +5581,10 @@
         <f t="shared" si="0"/>
         <v>331</v>
       </c>
-      <c r="E51" s="34"/>
+      <c r="E51" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F51" s="17">
         <f t="shared" si="1"/>
         <v>387</v>
@@ -5479,7 +5664,10 @@
         <f t="shared" si="0"/>
         <v>343</v>
       </c>
-      <c r="E52" s="34"/>
+      <c r="E52" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F52" s="17">
         <f t="shared" si="1"/>
         <v>325</v>
@@ -5559,7 +5747,10 @@
         <f t="shared" si="0"/>
         <v>259</v>
       </c>
-      <c r="E53" s="34"/>
+      <c r="E53" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F53" s="17">
         <f t="shared" si="1"/>
         <v>278</v>
@@ -5639,7 +5830,10 @@
         <f t="shared" si="0"/>
         <v>919</v>
       </c>
-      <c r="E54" s="34"/>
+      <c r="E54" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F54" s="17">
         <f t="shared" si="1"/>
         <v>545</v>
@@ -5719,7 +5913,10 @@
         <f t="shared" si="0"/>
         <v>472</v>
       </c>
-      <c r="E55" s="34"/>
+      <c r="E55" s="34">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
       <c r="F55" s="17">
         <f t="shared" si="1"/>
         <v>392</v>
@@ -5816,130 +6013,130 @@
       </c>
       <c r="E57" s="13">
         <f>SUM(E6:E55)</f>
-        <v>961</v>
+        <v>1634</v>
       </c>
       <c r="F57" s="20">
-        <f t="shared" ref="F57:AJ57" si="2">SUM(F6:F55)</f>
+        <f t="shared" ref="F57:AJ57" si="3">SUM(F6:F55)</f>
         <v>28136</v>
       </c>
       <c r="G57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9057</v>
       </c>
       <c r="H57" s="13">
-        <f t="shared" si="2"/>
-        <v>744</v>
+        <f t="shared" si="3"/>
+        <v>898</v>
       </c>
       <c r="I57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6365</v>
       </c>
       <c r="J57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9892</v>
       </c>
       <c r="K57" s="13">
-        <f t="shared" si="2"/>
-        <v>166</v>
+        <f t="shared" si="3"/>
+        <v>442</v>
       </c>
       <c r="L57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>8915</v>
       </c>
       <c r="M57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7302</v>
       </c>
       <c r="N57" s="13">
-        <f t="shared" si="2"/>
-        <v>43</v>
+        <f t="shared" si="3"/>
+        <v>188</v>
       </c>
       <c r="O57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6721</v>
       </c>
       <c r="P57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3706</v>
       </c>
       <c r="Q57" s="13">
-        <f t="shared" si="2"/>
-        <v>5</v>
+        <f t="shared" si="3"/>
+        <v>62</v>
       </c>
       <c r="R57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>3467</v>
       </c>
       <c r="S57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1817</v>
       </c>
       <c r="T57" s="13">
-        <f t="shared" si="2"/>
-        <v>1</v>
+        <f t="shared" si="3"/>
+        <v>35</v>
       </c>
       <c r="U57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1467</v>
       </c>
       <c r="V57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>836</v>
       </c>
       <c r="W57" s="13">
-        <f t="shared" si="2"/>
-        <v>2</v>
+        <f t="shared" si="3"/>
+        <v>7</v>
       </c>
       <c r="X57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>589</v>
       </c>
       <c r="Y57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>342</v>
       </c>
       <c r="Z57" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AA57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>270</v>
       </c>
       <c r="AB57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>96</v>
       </c>
       <c r="AC57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AD57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>168</v>
       </c>
       <c r="AE57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>38</v>
       </c>
       <c r="AF57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AG57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>97</v>
       </c>
       <c r="AH57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>12</v>
       </c>
       <c r="AI57" s="13">
-        <f t="shared" si="2"/>
-        <v>0</v>
+        <f t="shared" si="3"/>
+        <v>1</v>
       </c>
       <c r="AJ57" s="13">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>77</v>
       </c>
     </row>

</xml_diff>